<commit_message>
commiting few changes for the demo
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/simple.xlsx
+++ b/src/test/resources/testData/simple.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="5610" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="5610" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="qaTestSheetName" sheetId="18" r:id="rId1"/>
     <sheet name="uatTestSheetName" sheetId="17" r:id="rId2"/>
     <sheet name="stageTestSheetName" sheetId="16" r:id="rId3"/>
-    <sheet name="xprodTestSheetName" sheetId="19" r:id="rId4"/>
-    <sheet name="prodTestSheetName" sheetId="8" r:id="rId5"/>
+    <sheet name="prodTestSheetName" sheetId="19" r:id="rId4"/>
+    <sheet name="xxprodTestSheetName" sheetId="8" r:id="rId5"/>
     <sheet name="testLogo" sheetId="15" r:id="rId6"/>
     <sheet name="testSocialShareLinks" sheetId="9" r:id="rId7"/>
   </sheets>
@@ -796,7 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -905,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
some changes for demo
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/simple.xlsx
+++ b/src/test/resources/testData/simple.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="5610" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13665" windowHeight="5610" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="qaTestSheetName" sheetId="18" r:id="rId1"/>
     <sheet name="uatTestSheetName" sheetId="17" r:id="rId2"/>
     <sheet name="stageTestSheetName" sheetId="16" r:id="rId3"/>
-    <sheet name="prodTestSheetName" sheetId="19" r:id="rId4"/>
-    <sheet name="xxprodTestSheetName" sheetId="8" r:id="rId5"/>
+    <sheet name="xprodTestSheetName" sheetId="19" r:id="rId4"/>
+    <sheet name="prodTestSheetName" sheetId="8" r:id="rId5"/>
     <sheet name="testLogo" sheetId="15" r:id="rId6"/>
     <sheet name="testSocialShareLinks" sheetId="9" r:id="rId7"/>
   </sheets>
@@ -796,7 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -905,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>